<commit_message>
fix bug of 'NaN' lines in RequestDB
</commit_message>
<xml_diff>
--- a/PrinterWatch/excel_sheets/recent_model_stats.xlsx
+++ b/PrinterWatch/excel_sheets/recent_model_stats.xlsx
@@ -534,42 +534,42 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>400.0</t>
+          <t>420.0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>730.0</t>
+          <t>790.0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>4834.0</t>
+          <t>4904.0</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>5466.0</t>
+          <t>5751.0</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>7.779</t>
+          <t>7.24</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>4.560</t>
+          <t>4.390</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>13.590</t>
+          <t>12.148</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>15.062</t>
+          <t>14.064</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -579,17 +579,17 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0.098</t>
+          <t>0.100</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2690.515</t>
+          <t>2545.737</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>744.143</t>
+          <t>729.648</t>
         </is>
       </c>
     </row>
@@ -612,62 +612,62 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>490.0</t>
+          <t>540.0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1300.0</t>
+          <t>1460.0</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2174.0</t>
+          <t>2475.0</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>6567.0</t>
+          <t>7303.0</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>9.64</t>
+          <t>9.459</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>8.290</t>
+          <t>8.299</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>3.610</t>
+          <t>3.525</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>11.499</t>
+          <t>11.387</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0.035</t>
+          <t>0.034</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>0.152</t>
+          <t>0.151</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>2629.790</t>
+          <t>2520.095</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>565.027</t>
+          <t>568.193</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0.36</t>
+          <t>0.32</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -720,7 +720,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>21.84</t>
+          <t>19.79</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>invalid</t>
+          <t>89.0</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>invalid</t>
+          <t>15202.0</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>invalid</t>
+          <t>1.28</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>invalid</t>
+          <t>220.31</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>invalid</t>
+          <t>0.006</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>invalid</t>
+          <t>17080.89</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -944,22 +944,22 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0.41</t>
+          <t>0.36</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0.34</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>28.87</t>
+          <t>25.66</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>79.92</t>
+          <t>71.04</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1002,42 +1002,42 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>64.0</t>
+          <t>68.0</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>94.0</t>
+          <t>99.0</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>8044.0</t>
+          <t>8579.0</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>12770.0</t>
+          <t>13618.0</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1.24</t>
+          <t>1.140</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>0.590</t>
+          <t>0.54</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>77.805</t>
+          <t>72.75</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>122.179</t>
+          <t>114.445</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1052,12 +1052,12 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>35485.985</t>
+          <t>34776.575</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>13472.135</t>
+          <t>13740.24</t>
         </is>
       </c>
     </row>
@@ -1080,27 +1080,27 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>16.0</t>
+          <t>20.0</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>74.0</t>
+          <t>85.0</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>645.0</t>
+          <t>649.0</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>8706.0</t>
+          <t>10242.0</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.28</t>
+          <t>0.31</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1110,12 +1110,12 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>11.51</t>
+          <t>10.3</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>155.46</t>
+          <t>162.57</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1130,12 +1130,12 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>58443.75</t>
+          <t>54455.0</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>11764.86</t>
+          <t>12049.41</t>
         </is>
       </c>
     </row>
@@ -1158,42 +1158,42 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>31.0</t>
+          <t>34.0</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>78.0</t>
+          <t>89.0</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1737.0</t>
+          <t>2016.0</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>1974.0</t>
+          <t>2229.0</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>0.82</t>
+          <t>0.77</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0.68</t>
+          <t>0.67</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>9.453</t>
+          <t>9.416</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>10.814</t>
+          <t>10.434</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1203,17 +1203,17 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>0.054</t>
+          <t>0.053</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>11315.554</t>
+          <t>11467.617</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>3614.332</t>
+          <t>3632.269</t>
         </is>
       </c>
     </row>
@@ -1329,47 +1329,47 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>88.0</t>
+          <t>114.0</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>0.37</t>
+          <t>0.32</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>0.05</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>3.85</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>1.62</t>
+          <t>1.86</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>0.033</t>
+          <t>0.031</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>0.08</t>
+          <t>0.061</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>1480.0</t>
+          <t>1610.0</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>880.0</t>
+          <t>1140.0</t>
         </is>
       </c>
     </row>
@@ -1392,7 +1392,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>90.0</t>
+          <t>110.0</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1402,52 +1402,52 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>1082.0</t>
+          <t>1235.0</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1608.0</t>
+          <t>1697.0</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>1.63</t>
+          <t>1.8</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>1.63</t>
+          <t>1.47</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>19.67</t>
+          <t>20.24</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>29.23</t>
+          <t>27.81</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>0.016</t>
+          <t>0.018</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>0.117</t>
+          <t>0.111</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>2988.88</t>
+          <t>2665.45</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>595.55</t>
+          <t>628.51</t>
         </is>
       </c>
     </row>
@@ -1485,27 +1485,27 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>778.0</t>
+          <t>786.0</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0.36</t>
+          <t>0.32</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0.42</t>
+          <t>0.38</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>0.78</t>
+          <t>0.7</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>14.14</t>
+          <t>12.88</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1515,17 +1515,17 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>0.094</t>
+          <t>0.093</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>4105.0</t>
+          <t>4145.0</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>1111.42</t>
+          <t>1122.85</t>
         </is>
       </c>
     </row>
@@ -1568,22 +1568,22 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>0.600</t>
+          <t>0.52</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>0.46</t>
+          <t>0.399</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>1.839</t>
+          <t>1.635</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>5.25</t>
+          <t>4.685</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1626,62 +1626,62 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>150.0</t>
+          <t>160.0</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>280.0</t>
+          <t>330.0</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>3035.0</t>
+          <t>3336.0</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2162.0</t>
+          <t>2365.0</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2.969</t>
+          <t>2.800</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>1.859</t>
+          <t>1.869</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>19.88</t>
+          <t>19.413</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>14.046</t>
+          <t>13.57</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>0.017</t>
+          <t>0.016</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>0.162</t>
+          <t>0.161</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>3067.916</t>
+          <t>3199.81</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>896.116</t>
+          <t>774.427</t>
         </is>
       </c>
     </row>
@@ -1714,7 +1714,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>179.0</t>
+          <t>197.0</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1724,7 +1724,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>0.08</t>
+          <t>0.07</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1734,7 +1734,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>3.58</t>
+          <t>3.51</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>0.021</t>
+          <t>0.019</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1754,7 +1754,7 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>4475.0</t>
+          <t>4925.0</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1782,42 +1782,42 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>200.0</t>
+          <t>230.0</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>320.0</t>
+          <t>340.0</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2195.0</t>
+          <t>2689.0</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2150.0</t>
+          <t>2230.0</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>4.029</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2.12</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>11.065</t>
+          <t>12.027</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>10.782</t>
+          <t>9.927</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1827,17 +1827,17 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>0.109</t>
+          <t>0.110</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>2004.54</t>
+          <t>1970.172</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>650.22</t>
+          <t>643.255</t>
         </is>
       </c>
     </row>

</xml_diff>